<commit_message>
Cambio de nombres para ser más ordenado
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_R_Posibles.xlsx
+++ b/SubRES_TMPL/SubRES_R_Posibles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4151DDC3-B8A8-4B60-8837-43060C5C1F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531D3233-6AE0-4373-BFC9-F15273AC3E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FC596A1D-735D-47D8-8E25-30449B5B17D4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FC596A1D-735D-47D8-8E25-30449B5B17D4}"/>
   </bookViews>
   <sheets>
     <sheet name="6. Reservas" sheetId="1" r:id="rId1"/>
@@ -30877,7 +30877,7 @@
   </sheetPr>
   <dimension ref="C4:N156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A123" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se agrego valor al lifting
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_R_Posibles.xlsx
+++ b/SubRES_TMPL/SubRES_R_Posibles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARMEN\Documents\GitHub\TIMES-UIS-v1-Nov\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95D7317-17A9-4B2B-B3FB-8400E2BF0124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FDA97E-BB4C-4F6A-A0EC-23E7D05D49E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FC596A1D-735D-47D8-8E25-30449B5B17D4}"/>
+    <workbookView xWindow="0" yWindow="615" windowWidth="20490" windowHeight="10905" activeTab="3" xr2:uid="{FC596A1D-735D-47D8-8E25-30449B5B17D4}"/>
   </bookViews>
   <sheets>
     <sheet name="6. Reservas" sheetId="1" r:id="rId1"/>
@@ -198,8 +198,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1994,7 +1992,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2522,7 +2520,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1628249055"/>
@@ -2581,7 +2579,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1628235327"/>
@@ -2623,7 +2621,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2660,7 +2658,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -30931,8 +30929,8 @@
   </sheetPr>
   <dimension ref="C4:AV156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P66" sqref="P66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31533,7 +31531,9 @@
         <f>+F24</f>
         <v>78.745472847807775</v>
       </c>
-      <c r="G37" s="19"/>
+      <c r="G37" s="19">
+        <v>2</v>
+      </c>
       <c r="H37" s="18">
         <v>1</v>
       </c>
@@ -31554,7 +31554,7 @@
         <v>182.43898142380363</v>
       </c>
       <c r="G38" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H38" s="18">
         <v>1</v>
@@ -31576,7 +31576,7 @@
         <v>1704.7107572435661</v>
       </c>
       <c r="G39" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H39" s="18">
         <v>1</v>
@@ -31598,7 +31598,7 @@
         <v>9.0910238045926182</v>
       </c>
       <c r="G40" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40" s="18">
         <v>1</v>
@@ -31626,7 +31626,7 @@
         <v>344.19190942154142</v>
       </c>
       <c r="G41" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H41" s="18">
         <v>1</v>
@@ -31756,7 +31756,7 @@
         <v>70.889484822558785</v>
       </c>
       <c r="G42" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H42" s="18">
         <v>1</v>
@@ -31885,7 +31885,9 @@
         <f t="shared" si="3"/>
         <v>231.41390643451217</v>
       </c>
-      <c r="G43" s="19"/>
+      <c r="G43" s="19">
+        <v>2</v>
+      </c>
       <c r="H43" s="18">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
COPIA 22 MARZO 11 AM
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_R_Posibles.xlsx
+++ b/SubRES_TMPL/SubRES_R_Posibles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARMEN\Documents\GitHub\TIMES-UIS-v1-Nov\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FDA97E-BB4C-4F6A-A0EC-23E7D05D49E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A35D70D-E824-461B-84D9-145428C837B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="615" windowWidth="20490" windowHeight="10905" activeTab="3" xr2:uid="{FC596A1D-735D-47D8-8E25-30449B5B17D4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FC596A1D-735D-47D8-8E25-30449B5B17D4}"/>
   </bookViews>
   <sheets>
     <sheet name="6. Reservas" sheetId="1" r:id="rId1"/>
@@ -1089,13 +1089,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0E+00"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="\Te\x\t"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -1574,7 +1574,7 @@
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -1582,14 +1582,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1649,11 +1649,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1713,7 +1713,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1724,7 +1724,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1735,7 +1735,7 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="13" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1809,22 +1809,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="169" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="21" fillId="6" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="21" fillId="6" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1992,7 +1992,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2520,7 +2520,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1628249055"/>
@@ -2579,7 +2579,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1628235327"/>
@@ -2621,7 +2621,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2658,7 +2658,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3406,7 +3406,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main Menu"/>
@@ -25248,7 +25248,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="IEA Data"/>
@@ -25383,7 +25383,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="COMM"/>
@@ -25918,25 +25918,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181F1CC8-2C56-4CAC-AD4A-B1AFE9FC8086}">
   <dimension ref="B3:AF79"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="K4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24:Z33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="8" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="34.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" customWidth="1"/>
+    <col min="20" max="20" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="J3" s="108" t="s">
         <v>48</v>
       </c>
@@ -25948,7 +25948,7 @@
       <c r="N3" s="109"/>
       <c r="O3" s="110"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="str">
         <f>'[3]5. Data'!D4</f>
         <v>PCI</v>
@@ -25978,7 +25978,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="str">
         <f>'[3]5. Data'!E5</f>
@@ -26010,7 +26010,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C6" t="str">
         <f>'[3]5. Data'!C6</f>
         <v>Energético</v>
@@ -26047,7 +26047,7 @@
         <v>0.31320569464899362</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="str">
         <f>'[3]5. Data'!B7</f>
         <v>GAS</v>
@@ -26089,7 +26089,7 @@
         <v>0.72257053291536055</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="str">
         <f>'[3]5. Data'!B8</f>
         <v>LOIL</v>
@@ -26122,7 +26122,7 @@
         <v>3.6681127982646422</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="str">
         <f>'[3]5. Data'!B9</f>
         <v>MOIL</v>
@@ -26162,7 +26162,7 @@
         <v>1.0697811945594322</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="str">
         <f>'[3]5. Data'!B10</f>
         <v>HOIL</v>
@@ -26187,7 +26187,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="str">
         <f>'[3]5. Data'!B11</f>
         <v>GSL</v>
@@ -26212,7 +26212,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="str">
         <f>'[3]5. Data'!B12</f>
         <v>DSL</v>
@@ -26230,7 +26230,7 @@
         <v>75.166375708662926</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="str">
         <f>'[3]5. Data'!B13</f>
         <v>KER</v>
@@ -26249,7 +26249,7 @@
       </c>
       <c r="U13" s="11"/>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="str">
         <f>'[3]5. Data'!B14</f>
         <v>LPG</v>
@@ -26267,7 +26267,7 @@
         <v>47.28933824683137</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="str">
         <f>'[3]5. Data'!B15</f>
         <v>HFO</v>
@@ -26288,7 +26288,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="str">
         <f>'[3]5. Data'!B16</f>
         <v>AVG</v>
@@ -26327,7 +26327,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="str">
         <f>'[3]5. Data'!B17</f>
         <v>RFG</v>
@@ -26389,7 +26389,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="str">
         <f>'[3]5. Data'!B18</f>
         <v>*Para todos, menos gas natural, las unidades son TJ/Mpc; PJ/kpc</v>
@@ -26447,7 +26447,7 @@
       </c>
       <c r="AE18" s="48"/>
     </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J19" s="14" t="s">
         <v>4</v>
       </c>
@@ -26503,7 +26503,7 @@
         <v>1441.08</v>
       </c>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J20" s="14" t="s">
         <v>5</v>
       </c>
@@ -26559,7 +26559,7 @@
         <v>560.42000000000007</v>
       </c>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>6</v>
       </c>
@@ -26617,7 +26617,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -26677,7 +26677,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>5800</v>
       </c>
@@ -26720,7 +26720,7 @@
         <v>-238.875</v>
       </c>
     </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
       <c r="K24" s="12">
         <f t="shared" ref="K24:M24" si="5">+SUM(K18:K23)</f>
         <v>2084</v>
@@ -26771,7 +26771,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
       <c r="X25" t="s">
         <v>59</v>
       </c>
@@ -26785,7 +26785,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J26" t="s">
         <v>13</v>
       </c>
@@ -26848,7 +26848,7 @@
         <v>0.38352133398724864</v>
       </c>
     </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J27" t="s">
         <v>14</v>
       </c>
@@ -26919,7 +26919,7 @@
         <v>1688.3259911894272</v>
       </c>
     </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
         <v>15</v>
       </c>
@@ -26965,7 +26965,7 @@
         <v>0.31868131868131866</v>
       </c>
     </row>
-    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
         <v>16</v>
       </c>
@@ -27011,7 +27011,7 @@
         <v>0.1695447409733124</v>
       </c>
     </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J30" t="s">
         <v>17</v>
       </c>
@@ -27063,7 +27063,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:32" x14ac:dyDescent="0.3">
       <c r="X31" t="s">
         <v>59</v>
       </c>
@@ -27074,7 +27074,7 @@
         <v>3164</v>
       </c>
     </row>
-    <row r="32" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:32" x14ac:dyDescent="0.3">
       <c r="X32" t="s">
         <v>60</v>
       </c>
@@ -27093,7 +27093,7 @@
         <v>0.21744627054361568</v>
       </c>
     </row>
-    <row r="33" spans="24:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="24:29" x14ac:dyDescent="0.3">
       <c r="X33" t="s">
         <v>61</v>
       </c>
@@ -27112,7 +27112,7 @@
         <v>0.42003792667509482</v>
       </c>
     </row>
-    <row r="54" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="10:25" x14ac:dyDescent="0.3">
       <c r="R54" s="17" t="e">
         <f>+R57/(R57+S57)</f>
         <v>#DIV/0!</v>
@@ -27122,14 +27122,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="10:25" x14ac:dyDescent="0.3">
       <c r="Q55" s="1"/>
       <c r="R55" s="19" t="s">
         <v>18</v>
       </c>
       <c r="S55" s="19"/>
     </row>
-    <row r="56" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J56" s="1"/>
       <c r="K56" s="1" t="s">
         <v>18</v>
@@ -27151,7 +27151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J57" s="1" t="s">
         <v>24</v>
       </c>
@@ -27171,7 +27171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J58" s="1" t="s">
         <v>25</v>
       </c>
@@ -27193,7 +27193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="10:25" x14ac:dyDescent="0.3">
       <c r="Q62" t="s">
         <v>26</v>
       </c>
@@ -27201,7 +27201,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="10:25" x14ac:dyDescent="0.3">
       <c r="R63" t="s">
         <v>30</v>
       </c>
@@ -27221,7 +27221,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="10:25" x14ac:dyDescent="0.3">
       <c r="Q64" t="s">
         <v>34</v>
       </c>
@@ -27250,7 +27250,7 @@
         <v>16.15291750724262</v>
       </c>
     </row>
-    <row r="65" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="10:25" x14ac:dyDescent="0.3">
       <c r="Q65" t="s">
         <v>36</v>
       </c>
@@ -27279,7 +27279,7 @@
         <v>231.18863182241</v>
       </c>
     </row>
-    <row r="66" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="10:25" x14ac:dyDescent="0.3">
       <c r="Q66" t="s">
         <v>38</v>
       </c>
@@ -27308,7 +27308,7 @@
         <v>22.210261572458602</v>
       </c>
     </row>
-    <row r="67" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="10:25" x14ac:dyDescent="0.3">
       <c r="Q67" t="s">
         <v>40</v>
       </c>
@@ -27337,7 +27337,7 @@
         <v>73.697686126794451</v>
       </c>
     </row>
-    <row r="68" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="10:25" x14ac:dyDescent="0.3">
       <c r="Q68" t="s">
         <v>42</v>
       </c>
@@ -27366,7 +27366,7 @@
         <v>56.53521127534917</v>
       </c>
     </row>
-    <row r="70" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J70" t="s">
         <v>43</v>
       </c>
@@ -27387,7 +27387,7 @@
         <v>399.78470830425488</v>
       </c>
     </row>
-    <row r="71" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J71" t="s">
         <v>44</v>
       </c>
@@ -27396,7 +27396,7 @@
         <v>157.74</v>
       </c>
     </row>
-    <row r="72" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J72" t="s">
         <v>45</v>
       </c>
@@ -27404,7 +27404,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J73" t="s">
         <v>46</v>
       </c>
@@ -27412,20 +27412,20 @@
         <v>7.45</v>
       </c>
     </row>
-    <row r="75" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="10:25" x14ac:dyDescent="0.3">
       <c r="K75">
         <f>+K71+K70</f>
         <v>1019.86</v>
       </c>
       <c r="T75" s="22"/>
     </row>
-    <row r="76" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="10:25" x14ac:dyDescent="0.3">
       <c r="T76" s="22"/>
     </row>
-    <row r="77" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="10:25" x14ac:dyDescent="0.3">
       <c r="T77" s="22"/>
     </row>
-    <row r="78" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J78" t="s">
         <v>21</v>
       </c>
@@ -27442,7 +27442,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="79" spans="10:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="10:25" x14ac:dyDescent="0.3">
       <c r="J79" t="s">
         <v>47</v>
       </c>
@@ -27479,15 +27479,15 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>75</v>
       </c>
@@ -27495,13 +27495,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>78</v>
       </c>
@@ -27525,7 +27525,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -27539,7 +27539,7 @@
         <v>55.539114956987063</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>83</v>
       </c>
@@ -27569,7 +27569,7 @@
       <c r="W8" s="112"/>
       <c r="X8" s="112"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>85</v>
       </c>
@@ -27625,7 +27625,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
@@ -27691,7 +27691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
@@ -27758,7 +27758,7 @@
         <v>0.38366595333723663</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>91</v>
       </c>
@@ -27825,7 +27825,7 @@
         <v>0.3094426038072563</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
@@ -27884,7 +27884,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>95</v>
       </c>
@@ -27947,7 +27947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>97</v>
       </c>
@@ -28015,7 +28015,7 @@
         <v>0.38366595333723669</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>99</v>
       </c>
@@ -28081,7 +28081,7 @@
         <v>0.3094426038072563</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>101</v>
       </c>
@@ -28095,14 +28095,14 @@
         <v>40.784041574326501</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>103</v>
       </c>
       <c r="P18" s="41"/>
       <c r="Q18" s="41"/>
     </row>
-    <row r="19" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="I19" s="88" t="s">
         <v>63</v>
       </c>
@@ -28122,7 +28122,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -28154,7 +28154,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>6</v>
       </c>
@@ -28192,7 +28192,7 @@
         <v>371.21365467918736</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>5800</v>
       </c>
@@ -28226,7 +28226,7 @@
         <v>1811.5699899567956</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H23" s="71" t="s">
         <v>106</v>
       </c>
@@ -28253,7 +28253,7 @@
         <v>18.163324950452385</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H24" s="71" t="s">
         <v>107</v>
       </c>
@@ -28280,7 +28280,7 @@
         <v>10.016252198105461</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H25" s="71" t="s">
         <v>108</v>
       </c>
@@ -28308,7 +28308,7 @@
         <v>145.41673938682757</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H26" s="70" t="s">
         <v>109</v>
       </c>
@@ -28336,7 +28336,7 @@
         <v>13.800688062315521</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H27" s="70" t="s">
         <v>110</v>
       </c>
@@ -28364,7 +28364,7 @@
         <v>378.41110039157945</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I28" s="38">
         <f>+SUM(I21:I27)</f>
         <v>2000.5305040455908</v>
@@ -28382,13 +28382,13 @@
         <v>767</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K29" s="38"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K30" s="38"/>
     </row>
-    <row r="37" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H37" s="113" t="s">
         <v>117</v>
       </c>
@@ -28400,7 +28400,7 @@
       <c r="N37" s="113"/>
       <c r="O37" s="113"/>
     </row>
-    <row r="38" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I38" s="74" t="s">
         <v>30</v>
       </c>
@@ -28420,7 +28420,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H39" t="s">
         <v>34</v>
       </c>
@@ -28443,7 +28443,7 @@
         <v>3.9024390243902439E-2</v>
       </c>
     </row>
-    <row r="40" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
         <v>36</v>
       </c>
@@ -28466,7 +28466,7 @@
         <v>0.55853658536585371</v>
       </c>
     </row>
-    <row r="41" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H41" t="s">
         <v>38</v>
       </c>
@@ -28489,7 +28489,7 @@
         <v>5.3658536585365853E-2</v>
       </c>
     </row>
-    <row r="42" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H42" t="s">
         <v>40</v>
       </c>
@@ -28512,7 +28512,7 @@
         <v>0.17804878048780487</v>
       </c>
     </row>
-    <row r="43" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
         <v>42</v>
       </c>
@@ -28535,7 +28535,7 @@
         <v>0.13658536585365855</v>
       </c>
     </row>
-    <row r="44" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
         <v>118</v>
       </c>
@@ -28558,7 +28558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H45" t="s">
         <v>119</v>
       </c>
@@ -28575,7 +28575,7 @@
       <c r="M45" s="62"/>
       <c r="N45" s="76"/>
     </row>
-    <row r="46" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H46" t="s">
         <v>120</v>
       </c>
@@ -28599,7 +28599,7 @@
       </c>
       <c r="R46" s="41"/>
     </row>
-    <row r="47" spans="8:23" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:23" ht="18" x14ac:dyDescent="0.3">
       <c r="H47" t="s">
         <v>121</v>
       </c>
@@ -28630,7 +28630,7 @@
       </c>
       <c r="W47" s="22"/>
     </row>
-    <row r="48" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H48" t="s">
         <v>122</v>
       </c>
@@ -28661,7 +28661,7 @@
       </c>
       <c r="W48" s="22"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="H49" s="1" t="s">
         <v>123</v>
       </c>
@@ -28695,7 +28695,7 @@
       </c>
       <c r="W49" s="22"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="I50" s="54">
         <v>1</v>
       </c>
@@ -28718,7 +28718,7 @@
       </c>
       <c r="W50" s="22"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R51" s="84"/>
       <c r="S51" s="84"/>
       <c r="T51" s="22"/>
@@ -28728,7 +28728,7 @@
       </c>
       <c r="W51" s="22"/>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R52" s="84"/>
       <c r="S52" s="84"/>
       <c r="T52" s="22"/>
@@ -28738,7 +28738,7 @@
       </c>
       <c r="W52" s="22"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R53" s="84"/>
       <c r="S53" s="84"/>
       <c r="T53" s="22"/>
@@ -28748,7 +28748,7 @@
       </c>
       <c r="W53" s="22"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R54" s="84"/>
       <c r="S54" s="84"/>
       <c r="T54" s="22"/>
@@ -28758,7 +28758,7 @@
       </c>
       <c r="W54" s="22"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R55" s="84"/>
       <c r="S55" s="84"/>
       <c r="T55" s="22"/>
@@ -28770,22 +28770,22 @@
       <c r="W55" s="84"/>
       <c r="X55" s="38"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="W56" s="11"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="22"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" s="22"/>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
     </row>
-    <row r="60" spans="1:24" ht="21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:24" ht="21" x14ac:dyDescent="0.4">
       <c r="A60" s="22"/>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
@@ -28800,7 +28800,7 @@
       <c r="V60" s="111"/>
       <c r="W60" s="111"/>
     </row>
-    <row r="61" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="18" x14ac:dyDescent="0.3">
       <c r="A61" s="22"/>
       <c r="B61" s="22"/>
       <c r="C61" s="22"/>
@@ -28824,7 +28824,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="22"/>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
@@ -28852,7 +28852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="22"/>
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
@@ -28880,7 +28880,7 @@
         <v>0.70411500249785086</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R64" s="20">
         <f t="shared" si="15"/>
         <v>6496.7121983715815</v>
@@ -28904,7 +28904,7 @@
         <v>2.8224919834781794E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="R65" s="20">
         <f t="shared" si="15"/>
         <v>44.660401360000002</v>
@@ -28928,7 +28928,7 @@
         <v>0.2264193930205074</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" s="67"/>
       <c r="B66" s="67"/>
       <c r="C66" s="67"/>
@@ -28956,7 +28956,7 @@
         <v>2.9005932398423979E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="R67" s="20">
         <f t="shared" si="15"/>
         <v>283.33235609852005</v>
@@ -28980,7 +28980,7 @@
         <v>4.9174002504380532E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="R68" s="20">
         <f t="shared" si="15"/>
         <v>157.75252398843665</v>
@@ -29004,167 +29004,167 @@
         <v>0.99457310605335925</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V69" s="22"/>
       <c r="W69" s="85"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="22"/>
       <c r="B132" s="22"/>
       <c r="C132" s="22"/>
       <c r="D132" s="22"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="22"/>
       <c r="B133" s="22"/>
       <c r="C133" s="22"/>
       <c r="D133" s="22"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="22"/>
       <c r="B134" s="22"/>
       <c r="C134" s="22"/>
       <c r="D134" s="22"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="22"/>
       <c r="B135" s="22"/>
       <c r="C135" s="22"/>
       <c r="D135" s="22"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="22"/>
       <c r="B136" s="22"/>
       <c r="C136" s="22"/>
       <c r="D136" s="22"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="22"/>
       <c r="B137" s="22"/>
       <c r="C137" s="22"/>
       <c r="D137" s="22"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="22"/>
       <c r="B138" s="22"/>
       <c r="C138" s="22"/>
       <c r="D138" s="22"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="22"/>
       <c r="B139" s="22"/>
       <c r="C139" s="22"/>
       <c r="D139" s="22"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="22"/>
       <c r="B140" s="22"/>
       <c r="C140" s="22"/>
       <c r="D140" s="22"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="22"/>
       <c r="B141" s="22"/>
       <c r="C141" s="22"/>
       <c r="D141" s="22"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="22"/>
       <c r="B142" s="22"/>
       <c r="C142" s="22"/>
       <c r="D142" s="22"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="22"/>
       <c r="B143" s="22"/>
       <c r="C143" s="22"/>
       <c r="D143" s="22"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="22"/>
       <c r="B144" s="22"/>
       <c r="C144" s="22"/>
       <c r="D144" s="22"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="22"/>
       <c r="B145" s="22"/>
       <c r="C145" s="22"/>
       <c r="D145" s="22"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="22"/>
       <c r="B146" s="22"/>
       <c r="C146" s="22"/>
       <c r="D146" s="22"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="22"/>
       <c r="B147" s="22"/>
       <c r="C147" s="22"/>
       <c r="D147" s="22"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="22"/>
       <c r="B148" s="22"/>
       <c r="C148" s="22"/>
       <c r="D148" s="22"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="22"/>
       <c r="B149" s="22"/>
       <c r="C149" s="22"/>
       <c r="D149" s="22"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="22"/>
       <c r="B150" s="22"/>
       <c r="C150" s="22"/>
       <c r="D150" s="22"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="22"/>
       <c r="B151" s="22"/>
       <c r="C151" s="22"/>
       <c r="D151" s="22"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="22"/>
       <c r="B152" s="22"/>
       <c r="C152" s="22"/>
       <c r="D152" s="22"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="22"/>
       <c r="B153" s="22"/>
       <c r="C153" s="22"/>
       <c r="D153" s="22"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="22"/>
       <c r="B154" s="22"/>
       <c r="C154" s="22"/>
       <c r="D154" s="22"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="22"/>
       <c r="B155" s="22"/>
       <c r="C155" s="22"/>
       <c r="D155" s="22"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="22"/>
       <c r="B156" s="22"/>
       <c r="C156" s="22"/>
       <c r="D156" s="22"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="22"/>
       <c r="B157" s="22"/>
       <c r="C157" s="22"/>
       <c r="D157" s="22"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="22"/>
       <c r="B158" s="22"/>
       <c r="C158" s="22"/>
@@ -29202,15 +29202,15 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>75</v>
       </c>
@@ -29218,13 +29218,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>78</v>
       </c>
@@ -29248,7 +29248,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -29262,7 +29262,7 @@
         <v>55.539114956987063</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>83</v>
       </c>
@@ -29292,7 +29292,7 @@
       <c r="W8" s="112"/>
       <c r="X8" s="112"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>85</v>
       </c>
@@ -29348,7 +29348,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
@@ -29414,7 +29414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
@@ -29481,7 +29481,7 @@
         <v>0.38366595333723663</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>91</v>
       </c>
@@ -29548,7 +29548,7 @@
         <v>0.3094426038072563</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
@@ -29607,7 +29607,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>95</v>
       </c>
@@ -29670,7 +29670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>97</v>
       </c>
@@ -29738,7 +29738,7 @@
         <v>0.38366595333723669</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>99</v>
       </c>
@@ -29804,7 +29804,7 @@
         <v>0.3094426038072563</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>101</v>
       </c>
@@ -29818,14 +29818,14 @@
         <v>40.784041574326501</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>103</v>
       </c>
       <c r="P18" s="41"/>
       <c r="Q18" s="41"/>
     </row>
-    <row r="19" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="I19" s="88" t="s">
         <v>63</v>
       </c>
@@ -29845,7 +29845,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -29877,7 +29877,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>6</v>
       </c>
@@ -29915,7 +29915,7 @@
         <v>342.21365467918736</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>5800</v>
       </c>
@@ -29949,7 +29949,7 @@
         <v>1505.5699899567956</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H23" s="71" t="s">
         <v>106</v>
       </c>
@@ -29976,7 +29976,7 @@
         <v>18.163324950452385</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H24" s="71" t="s">
         <v>107</v>
       </c>
@@ -30003,7 +30003,7 @@
         <v>10.016252198105461</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H25" s="71" t="s">
         <v>108</v>
       </c>
@@ -30031,7 +30031,7 @@
         <v>103.41673938682757</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H26" s="70" t="s">
         <v>109</v>
       </c>
@@ -30059,7 +30059,7 @@
         <v>13.800688062315521</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H27" s="70" t="s">
         <v>110</v>
       </c>
@@ -30087,7 +30087,7 @@
         <v>384.41110039157945</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I28" s="38">
         <f>+SUM(I21:I27)</f>
         <v>2000.5305040455908</v>
@@ -30113,13 +30113,13 @@
         <v>2377.5917496252632</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K29" s="38"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K30" s="38"/>
     </row>
-    <row r="37" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H37" s="113" t="s">
         <v>117</v>
       </c>
@@ -30131,7 +30131,7 @@
       <c r="N37" s="113"/>
       <c r="O37" s="113"/>
     </row>
-    <row r="38" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I38" s="74" t="s">
         <v>30</v>
       </c>
@@ -30151,7 +30151,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H39" t="s">
         <v>34</v>
       </c>
@@ -30174,7 +30174,7 @@
         <v>3.9024390243902439E-2</v>
       </c>
     </row>
-    <row r="40" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
         <v>36</v>
       </c>
@@ -30197,7 +30197,7 @@
         <v>0.55853658536585371</v>
       </c>
     </row>
-    <row r="41" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H41" t="s">
         <v>38</v>
       </c>
@@ -30220,7 +30220,7 @@
         <v>5.3658536585365853E-2</v>
       </c>
     </row>
-    <row r="42" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H42" t="s">
         <v>40</v>
       </c>
@@ -30243,7 +30243,7 @@
         <v>0.17804878048780487</v>
       </c>
     </row>
-    <row r="43" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
         <v>42</v>
       </c>
@@ -30266,7 +30266,7 @@
         <v>0.13658536585365855</v>
       </c>
     </row>
-    <row r="44" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
         <v>118</v>
       </c>
@@ -30289,7 +30289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H45" t="s">
         <v>119</v>
       </c>
@@ -30306,7 +30306,7 @@
       <c r="M45" s="62"/>
       <c r="N45" s="76"/>
     </row>
-    <row r="46" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H46" t="s">
         <v>120</v>
       </c>
@@ -30330,7 +30330,7 @@
       </c>
       <c r="R46" s="41"/>
     </row>
-    <row r="47" spans="8:23" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:23" ht="18" x14ac:dyDescent="0.3">
       <c r="H47" t="s">
         <v>121</v>
       </c>
@@ -30361,7 +30361,7 @@
       </c>
       <c r="W47" s="22"/>
     </row>
-    <row r="48" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H48" t="s">
         <v>122</v>
       </c>
@@ -30392,7 +30392,7 @@
       </c>
       <c r="W48" s="22"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="H49" s="1" t="s">
         <v>123</v>
       </c>
@@ -30426,7 +30426,7 @@
       </c>
       <c r="W49" s="22"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="I50" s="54">
         <v>1</v>
       </c>
@@ -30449,7 +30449,7 @@
       </c>
       <c r="W50" s="22"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R51" s="84"/>
       <c r="S51" s="84"/>
       <c r="T51" s="22"/>
@@ -30459,7 +30459,7 @@
       </c>
       <c r="W51" s="22"/>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R52" s="84"/>
       <c r="S52" s="84"/>
       <c r="T52" s="22"/>
@@ -30469,7 +30469,7 @@
       </c>
       <c r="W52" s="22"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R53" s="84"/>
       <c r="S53" s="84"/>
       <c r="T53" s="22"/>
@@ -30479,7 +30479,7 @@
       </c>
       <c r="W53" s="22"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R54" s="84"/>
       <c r="S54" s="84"/>
       <c r="T54" s="22"/>
@@ -30489,7 +30489,7 @@
       </c>
       <c r="W54" s="22"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R55" s="84"/>
       <c r="S55" s="84"/>
       <c r="T55" s="22"/>
@@ -30501,22 +30501,22 @@
       <c r="W55" s="84"/>
       <c r="X55" s="38"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="W56" s="11"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="22"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" s="22"/>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
     </row>
-    <row r="60" spans="1:24" ht="21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:24" ht="21" x14ac:dyDescent="0.4">
       <c r="A60" s="22"/>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
@@ -30531,7 +30531,7 @@
       <c r="V60" s="111"/>
       <c r="W60" s="111"/>
     </row>
-    <row r="61" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="18" x14ac:dyDescent="0.3">
       <c r="A61" s="22"/>
       <c r="B61" s="22"/>
       <c r="C61" s="22"/>
@@ -30555,7 +30555,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="22"/>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
@@ -30583,7 +30583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="22"/>
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
@@ -30611,7 +30611,7 @@
         <v>0.70411500249785086</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="R64" s="20">
         <f t="shared" si="13"/>
         <v>6496.7121983715815</v>
@@ -30635,7 +30635,7 @@
         <v>2.8224919834781794E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="R65" s="20">
         <f t="shared" si="13"/>
         <v>44.660401360000002</v>
@@ -30659,7 +30659,7 @@
         <v>0.2264193930205074</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" s="67"/>
       <c r="B66" s="67"/>
       <c r="C66" s="67"/>
@@ -30687,7 +30687,7 @@
         <v>2.9005932398423979E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="R67" s="20">
         <f t="shared" si="13"/>
         <v>283.33235609852005</v>
@@ -30711,7 +30711,7 @@
         <v>4.9174002504380532E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="R68" s="20">
         <f t="shared" si="13"/>
         <v>157.75252398843665</v>
@@ -30735,167 +30735,167 @@
         <v>0.99457310605335925</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V69" s="22"/>
       <c r="W69" s="85"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="22"/>
       <c r="B132" s="22"/>
       <c r="C132" s="22"/>
       <c r="D132" s="22"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="22"/>
       <c r="B133" s="22"/>
       <c r="C133" s="22"/>
       <c r="D133" s="22"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="22"/>
       <c r="B134" s="22"/>
       <c r="C134" s="22"/>
       <c r="D134" s="22"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="22"/>
       <c r="B135" s="22"/>
       <c r="C135" s="22"/>
       <c r="D135" s="22"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="22"/>
       <c r="B136" s="22"/>
       <c r="C136" s="22"/>
       <c r="D136" s="22"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="22"/>
       <c r="B137" s="22"/>
       <c r="C137" s="22"/>
       <c r="D137" s="22"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="22"/>
       <c r="B138" s="22"/>
       <c r="C138" s="22"/>
       <c r="D138" s="22"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="22"/>
       <c r="B139" s="22"/>
       <c r="C139" s="22"/>
       <c r="D139" s="22"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="22"/>
       <c r="B140" s="22"/>
       <c r="C140" s="22"/>
       <c r="D140" s="22"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="22"/>
       <c r="B141" s="22"/>
       <c r="C141" s="22"/>
       <c r="D141" s="22"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="22"/>
       <c r="B142" s="22"/>
       <c r="C142" s="22"/>
       <c r="D142" s="22"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="22"/>
       <c r="B143" s="22"/>
       <c r="C143" s="22"/>
       <c r="D143" s="22"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="22"/>
       <c r="B144" s="22"/>
       <c r="C144" s="22"/>
       <c r="D144" s="22"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="22"/>
       <c r="B145" s="22"/>
       <c r="C145" s="22"/>
       <c r="D145" s="22"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="22"/>
       <c r="B146" s="22"/>
       <c r="C146" s="22"/>
       <c r="D146" s="22"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="22"/>
       <c r="B147" s="22"/>
       <c r="C147" s="22"/>
       <c r="D147" s="22"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="22"/>
       <c r="B148" s="22"/>
       <c r="C148" s="22"/>
       <c r="D148" s="22"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="22"/>
       <c r="B149" s="22"/>
       <c r="C149" s="22"/>
       <c r="D149" s="22"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="22"/>
       <c r="B150" s="22"/>
       <c r="C150" s="22"/>
       <c r="D150" s="22"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="22"/>
       <c r="B151" s="22"/>
       <c r="C151" s="22"/>
       <c r="D151" s="22"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="22"/>
       <c r="B152" s="22"/>
       <c r="C152" s="22"/>
       <c r="D152" s="22"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="22"/>
       <c r="B153" s="22"/>
       <c r="C153" s="22"/>
       <c r="D153" s="22"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="22"/>
       <c r="B154" s="22"/>
       <c r="C154" s="22"/>
       <c r="D154" s="22"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="22"/>
       <c r="B155" s="22"/>
       <c r="C155" s="22"/>
       <c r="D155" s="22"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="22"/>
       <c r="B156" s="22"/>
       <c r="C156" s="22"/>
       <c r="D156" s="22"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="22"/>
       <c r="B157" s="22"/>
       <c r="C157" s="22"/>
       <c r="D157" s="22"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="22"/>
       <c r="B158" s="22"/>
       <c r="C158" s="22"/>
@@ -30929,20 +30929,20 @@
   </sheetPr>
   <dimension ref="C4:AV156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="5" width="20.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="5" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="16" max="16" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:14" ht="21" x14ac:dyDescent="0.4">
       <c r="C4" s="111" t="s">
         <v>65</v>
       </c>
@@ -30952,7 +30952,7 @@
       <c r="G4" s="111"/>
       <c r="H4" s="111"/>
     </row>
-    <row r="6" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="49"/>
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
@@ -30960,12 +30960,12 @@
       <c r="G6" s="49"/>
       <c r="H6" s="49"/>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C7" s="50" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="3:14" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="C9" s="51" t="s">
         <v>67</v>
       </c>
@@ -30997,7 +30997,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>146</v>
       </c>
@@ -31031,7 +31031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>134</v>
       </c>
@@ -31065,7 +31065,7 @@
         <v>166.28606391656101</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>136</v>
       </c>
@@ -31099,7 +31099,7 @@
         <v>1704.7107572435661</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>138</v>
       </c>
@@ -31133,7 +31133,7 @@
         <v>9.0910238045926182</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>140</v>
       </c>
@@ -31167,7 +31167,7 @@
         <v>270.49422329474697</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>142</v>
       </c>
@@ -31201,7 +31201,7 @@
         <v>70.889484822558785</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>144</v>
       </c>
@@ -31235,7 +31235,7 @@
         <v>0.22527461210215591</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="19"/>
@@ -31252,7 +31252,7 @@
       </c>
       <c r="L17" s="16"/>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F19" s="38">
         <f>+SUM(F10:F16)</f>
         <v>10443.59672371719</v>
@@ -31274,7 +31274,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
       <c r="J20" t="s">
         <v>150</v>
       </c>
@@ -31293,7 +31293,7 @@
         <v>0.26313862403658173</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C21" s="50" t="s">
         <v>153</v>
       </c>
@@ -31305,7 +31305,7 @@
         <v>2621.4815359983822</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C23" s="51" t="s">
         <v>67</v>
       </c>
@@ -31325,7 +31325,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C24" s="19" t="str" cm="1">
         <f t="array" ref="C24:C30">+C37:C43</f>
         <v>MIN-P3-CAM1</v>
@@ -31350,7 +31350,7 @@
       </c>
       <c r="L24" s="16"/>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C25" s="19" t="str">
         <v>MIN-P3-CAM2</v>
       </c>
@@ -31372,7 +31372,7 @@
       </c>
       <c r="L25" s="16"/>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C26" s="19" t="str">
         <v>MIN-P3-CAM3</v>
       </c>
@@ -31394,7 +31394,7 @@
       </c>
       <c r="L26" s="16"/>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C27" s="19" t="str">
         <v>MIN-P3-CAM4</v>
       </c>
@@ -31416,7 +31416,7 @@
       </c>
       <c r="L27" s="16"/>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C28" s="19" t="str">
         <v>MIN-P3-CAM5</v>
       </c>
@@ -31438,7 +31438,7 @@
       </c>
       <c r="L28" s="16"/>
     </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C29" s="19" t="str">
         <v>MIN-P3-CAM6</v>
       </c>
@@ -31460,7 +31460,7 @@
       </c>
       <c r="L29" s="16"/>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C30" s="19" t="str">
         <v>MIN-P3-CAM7</v>
       </c>
@@ -31482,18 +31482,18 @@
       </c>
       <c r="L30" s="16"/>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.3">
       <c r="F32" s="20">
         <f>+SUM(F24:F30)</f>
         <v>2621.4815359983827</v>
       </c>
     </row>
-    <row r="35" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D35" s="107" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C36" s="51" t="s">
         <v>67</v>
       </c>
@@ -31516,7 +31516,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C37" s="19" t="str">
         <f>+D48</f>
         <v>MIN-P3-CAM1</v>
@@ -31538,7 +31538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C38" s="19" t="str">
         <f t="shared" ref="C38:C43" si="2">+D49</f>
         <v>MIN-P3-CAM2</v>
@@ -31560,7 +31560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C39" s="19" t="str">
         <f t="shared" si="2"/>
         <v>MIN-P3-CAM3</v>
@@ -31582,7 +31582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C40" s="19" t="str">
         <f t="shared" si="2"/>
         <v>MIN-P3-CAM4</v>
@@ -31610,7 +31610,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C41" s="19" t="str">
         <f t="shared" si="2"/>
         <v>MIN-P3-CAM5</v>
@@ -31740,7 +31740,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="42" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C42" s="19" t="str">
         <f t="shared" si="2"/>
         <v>MIN-P3-CAM6</v>
@@ -31870,7 +31870,7 @@
         <v>11.0719100573523</v>
       </c>
     </row>
-    <row r="43" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C43" s="19" t="str">
         <f t="shared" si="2"/>
         <v>MIN-P3-CAM7</v>
@@ -32000,7 +32000,7 @@
         <v>11.0719100573523</v>
       </c>
     </row>
-    <row r="44" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:48" x14ac:dyDescent="0.3">
       <c r="M44" t="s">
         <v>185</v>
       </c>
@@ -32110,7 +32110,7 @@
         <v>31.238687075339602</v>
       </c>
     </row>
-    <row r="45" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:48" x14ac:dyDescent="0.3">
       <c r="M45" t="s">
         <v>185</v>
       </c>
@@ -32220,7 +32220,7 @@
         <v>31.238687075339602</v>
       </c>
     </row>
-    <row r="46" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D46" s="102" t="s">
         <v>155</v>
       </c>
@@ -32306,7 +32306,7 @@
         <v>81.576079976983493</v>
       </c>
     </row>
-    <row r="47" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C47" s="104" t="s">
         <v>156</v>
       </c>
@@ -32419,7 +32419,7 @@
         <v>239.56071857838401</v>
       </c>
     </row>
-    <row r="48" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>160</v>
       </c>
@@ -32478,7 +32478,7 @@
         <v>2.01080412501886</v>
       </c>
     </row>
-    <row r="49" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>166</v>
       </c>
@@ -32543,7 +32543,7 @@
         <v>0.51150808288774097</v>
       </c>
     </row>
-    <row r="50" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>167</v>
       </c>
@@ -32620,7 +32620,7 @@
         <v>50.853389506252697</v>
       </c>
     </row>
-    <row r="51" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>168</v>
       </c>
@@ -32718,7 +32718,7 @@
         <v>13.4036279819246</v>
       </c>
     </row>
-    <row r="52" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>169</v>
       </c>
@@ -32810,7 +32810,7 @@
         <v>6.4300587317359703</v>
       </c>
     </row>
-    <row r="53" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>170</v>
       </c>
@@ -32920,7 +32920,7 @@
         <v>4.7594154055897198</v>
       </c>
     </row>
-    <row r="54" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
         <v>171</v>
       </c>
@@ -33042,7 +33042,7 @@
         <v>6.5119610393585496</v>
       </c>
     </row>
-    <row r="55" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:48" x14ac:dyDescent="0.3">
       <c r="M55" t="s">
         <v>185</v>
       </c>
@@ -33152,10 +33152,10 @@
         <v>6.5119610393585496</v>
       </c>
     </row>
-    <row r="57" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:48" x14ac:dyDescent="0.3">
       <c r="D57" s="107"/>
     </row>
-    <row r="58" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C58" s="51" t="s">
         <v>67</v>
       </c>
@@ -33178,7 +33178,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C59" s="19" t="str">
         <f>+D48</f>
         <v>MIN-P3-CAM1</v>
@@ -33216,7 +33216,7 @@
         <v>0.78124740176190743</v>
       </c>
     </row>
-    <row r="60" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C60" s="19"/>
       <c r="D60" s="19" t="s">
         <v>162</v>
@@ -33251,7 +33251,7 @@
         <v>0.99102804789693577</v>
       </c>
     </row>
-    <row r="61" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C61" s="19"/>
       <c r="D61" s="19" t="s">
         <v>162</v>
@@ -33286,7 +33286,7 @@
         <v>0.99822310952824411</v>
       </c>
     </row>
-    <row r="62" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C62" s="19"/>
       <c r="D62" s="19" t="s">
         <v>162</v>
@@ -33321,7 +33321,7 @@
         <v>0.77358060697949249</v>
       </c>
     </row>
-    <row r="63" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C63" s="19"/>
       <c r="D63" s="19" t="s">
         <v>162</v>
@@ -33356,7 +33356,7 @@
         <v>0.8713766862218344</v>
       </c>
     </row>
-    <row r="64" spans="3:48" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:48" x14ac:dyDescent="0.3">
       <c r="C64" s="19"/>
       <c r="D64" s="19" t="s">
         <v>162</v>
@@ -33391,7 +33391,7 @@
         <v>0.99191020232553662</v>
       </c>
     </row>
-    <row r="65" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C65" s="19"/>
       <c r="D65" s="19" t="s">
         <v>162</v>
@@ -33426,7 +33426,7 @@
         <v>0.41377094975710332</v>
       </c>
     </row>
-    <row r="66" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C66" s="19"/>
       <c r="D66" s="19" t="s">
         <v>162</v>
@@ -33438,7 +33438,7 @@
         <v>2.86729599242289</v>
       </c>
     </row>
-    <row r="67" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C67" s="19"/>
       <c r="D67" s="19" t="s">
         <v>162</v>
@@ -33450,7 +33450,7 @@
         <v>2.3371052350566992</v>
       </c>
     </row>
-    <row r="68" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C68" s="19"/>
       <c r="D68" s="19" t="s">
         <v>162</v>
@@ -33462,7 +33462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C69" s="19"/>
       <c r="D69" s="19" t="s">
         <v>162</v>
@@ -33474,7 +33474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C70" s="19"/>
       <c r="D70" s="19" t="s">
         <v>162</v>
@@ -33486,7 +33486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C71" s="19"/>
       <c r="D71" s="19" t="s">
         <v>162</v>
@@ -33498,7 +33498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C72" s="19"/>
       <c r="D72" s="19" t="s">
         <v>162</v>
@@ -33510,7 +33510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C73" s="19" t="str">
         <f>+D49</f>
         <v>MIN-P3-CAM2</v>
@@ -33529,7 +33529,7 @@
         <v>119.17281573814111</v>
       </c>
     </row>
-    <row r="74" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D74" s="19" t="s">
         <v>162</v>
       </c>
@@ -33540,7 +33540,7 @@
         <v>357.03963544887284</v>
       </c>
     </row>
-    <row r="75" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D75" s="19" t="s">
         <v>162</v>
       </c>
@@ -33551,7 +33551,7 @@
         <v>291.71333965512213</v>
       </c>
     </row>
-    <row r="76" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D76" s="19" t="s">
         <v>162</v>
       </c>
@@ -33562,7 +33562,7 @@
         <v>219.06541620476196</v>
       </c>
     </row>
-    <row r="77" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D77" s="19" t="s">
         <v>162</v>
       </c>
@@ -33573,7 +33573,7 @@
         <v>126.28578711913453</v>
       </c>
     </row>
-    <row r="78" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D78" s="19" t="s">
         <v>162</v>
       </c>
@@ -33584,7 +33584,7 @@
         <v>93.858549318283977</v>
       </c>
     </row>
-    <row r="79" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D79" s="19" t="s">
         <v>162</v>
       </c>
@@ -33595,7 +33595,7 @@
         <v>67.926190092891318</v>
       </c>
     </row>
-    <row r="80" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D80" s="19" t="s">
         <v>162</v>
       </c>
@@ -33606,7 +33606,7 @@
         <v>51.633133760529908</v>
       </c>
     </row>
-    <row r="81" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D81" s="19" t="s">
         <v>162</v>
       </c>
@@ -33617,7 +33617,7 @@
         <v>39.112638374469476</v>
       </c>
     </row>
-    <row r="82" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D82" s="19" t="s">
         <v>162</v>
       </c>
@@ -33628,7 +33628,7 @@
         <v>23.3968962245543</v>
       </c>
     </row>
-    <row r="83" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D83" s="19" t="s">
         <v>162</v>
       </c>
@@ -33639,7 +33639,7 @@
         <v>10.786632390437573</v>
       </c>
     </row>
-    <row r="84" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D84" s="19" t="s">
         <v>162</v>
       </c>
@@ -33650,7 +33650,7 @@
         <v>9.0936013935059616</v>
       </c>
     </row>
-    <row r="85" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D85" s="19" t="s">
         <v>162</v>
       </c>
@@ -33661,7 +33661,7 @@
         <v>8.1321048795691553</v>
       </c>
     </row>
-    <row r="86" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D86" s="19" t="s">
         <v>162</v>
       </c>
@@ -33672,7 +33672,7 @@
         <v>6.6898601086639449</v>
       </c>
     </row>
-    <row r="87" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C87" s="19" t="str">
         <f>+D50</f>
         <v>MIN-P3-CAM3</v>
@@ -33691,7 +33691,7 @@
         <v>257.2828390567538</v>
       </c>
     </row>
-    <row r="88" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D88" s="19" t="s">
         <v>162</v>
       </c>
@@ -33702,7 +33702,7 @@
         <v>687.86225103060212</v>
       </c>
     </row>
-    <row r="89" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D89" s="19" t="s">
         <v>162</v>
       </c>
@@ -33713,7 +33713,7 @@
         <v>385.85872204465466</v>
       </c>
     </row>
-    <row r="90" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D90" s="19" t="s">
         <v>162</v>
       </c>
@@ -33724,7 +33724,7 @@
         <v>409.06901747594299</v>
       </c>
     </row>
-    <row r="91" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D91" s="19" t="s">
         <v>162</v>
       </c>
@@ -33735,7 +33735,7 @@
         <v>369.35783750049205</v>
       </c>
     </row>
-    <row r="92" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D92" s="19" t="s">
         <v>162</v>
       </c>
@@ -33746,7 +33746,7 @@
         <v>309.7910675373156</v>
       </c>
     </row>
-    <row r="93" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D93" s="19" t="s">
         <v>162</v>
       </c>
@@ -33757,7 +33757,7 @@
         <v>196.2800040437545</v>
       </c>
     </row>
-    <row r="94" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D94" s="19" t="s">
         <v>162</v>
       </c>
@@ -33768,7 +33768,7 @@
         <v>151.73365907601499</v>
       </c>
     </row>
-    <row r="95" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D95" s="19" t="s">
         <v>162</v>
       </c>
@@ -33779,7 +33779,7 @@
         <v>35.113596160592415</v>
       </c>
     </row>
-    <row r="96" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D96" s="19" t="s">
         <v>162</v>
       </c>
@@ -33790,7 +33790,7 @@
         <v>85.07145902842241</v>
       </c>
     </row>
-    <row r="97" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D97" s="19" t="s">
         <v>162</v>
       </c>
@@ -33801,7 +33801,7 @@
         <v>76.155967420534168</v>
       </c>
     </row>
-    <row r="98" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D98" s="19" t="s">
         <v>162</v>
       </c>
@@ -33812,7 +33812,7 @@
         <v>62.622403033114466</v>
       </c>
     </row>
-    <row r="99" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D99" s="19" t="s">
         <v>162</v>
       </c>
@@ -33823,7 +33823,7 @@
         <v>58.552871897120902</v>
       </c>
     </row>
-    <row r="100" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D100" s="19" t="s">
         <v>162</v>
       </c>
@@ -33834,7 +33834,7 @@
         <v>47.786379701308284</v>
       </c>
     </row>
-    <row r="101" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C101" s="19" t="str">
         <f>+D51</f>
         <v>MIN-P3-CAM4</v>
@@ -33853,7 +33853,7 @@
         <v>2.3603684699303833</v>
       </c>
     </row>
-    <row r="102" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D102" s="19" t="s">
         <v>162</v>
       </c>
@@ -33864,7 +33864,7 @@
         <v>5.3251450871105153</v>
       </c>
     </row>
-    <row r="103" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D103" s="19" t="s">
         <v>162</v>
       </c>
@@ -33875,7 +33875,7 @@
         <v>4.6229281525464918</v>
       </c>
     </row>
-    <row r="104" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D104" s="19" t="s">
         <v>162</v>
       </c>
@@ -33886,7 +33886,7 @@
         <v>4.1547835295038089</v>
       </c>
     </row>
-    <row r="105" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D105" s="19" t="s">
         <v>162</v>
       </c>
@@ -33897,7 +33897,7 @@
         <v>3.4993810572440531</v>
       </c>
     </row>
-    <row r="106" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D106" s="19" t="s">
         <v>162</v>
       </c>
@@ -33908,7 +33908,7 @@
         <v>2.5162773488544192</v>
       </c>
     </row>
-    <row r="107" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D107" s="19" t="s">
         <v>162</v>
       </c>
@@ -33919,7 +33919,7 @@
         <v>2.0247254946596036</v>
       </c>
     </row>
-    <row r="108" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D108" s="19" t="s">
         <v>162</v>
       </c>
@@ -33930,7 +33930,7 @@
         <v>1.6970242585297266</v>
       </c>
     </row>
-    <row r="109" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D109" s="19" t="s">
         <v>162</v>
       </c>
@@ -33941,7 +33941,7 @@
         <v>1.4629519470083856</v>
       </c>
     </row>
-    <row r="110" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D110" s="19" t="s">
         <v>162</v>
       </c>
@@ -33952,7 +33952,7 @@
         <v>1.1118434797263739</v>
       </c>
     </row>
-    <row r="111" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D111" s="19" t="s">
         <v>162</v>
       </c>
@@ -33963,7 +33963,7 @@
         <v>0.99480732396570282</v>
       </c>
     </row>
-    <row r="112" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D112" s="19" t="s">
         <v>162</v>
       </c>
@@ -33974,7 +33974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D113" s="19" t="s">
         <v>162</v>
       </c>
@@ -33985,7 +33985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D114" s="19" t="s">
         <v>162</v>
       </c>
@@ -33996,7 +33996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C115" s="19" t="str">
         <f>+D52</f>
         <v>MIN-P3-CAM5</v>
@@ -34015,7 +34015,7 @@
         <v>54.291427485409322</v>
       </c>
     </row>
-    <row r="116" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D116" s="19" t="s">
         <v>162</v>
       </c>
@@ -34026,7 +34026,7 @@
         <v>153.89107121101256</v>
       </c>
     </row>
-    <row r="117" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D117" s="19" t="s">
         <v>162</v>
       </c>
@@ -34037,7 +34037,7 @@
         <v>98.967477778380101</v>
       </c>
     </row>
-    <row r="118" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D118" s="19" t="s">
         <v>162</v>
       </c>
@@ -34048,7 +34048,7 @@
         <v>91.230677358831571</v>
       </c>
     </row>
-    <row r="119" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D119" s="19" t="s">
         <v>162</v>
       </c>
@@ -34059,7 +34059,7 @@
         <v>73.193552767530946</v>
       </c>
     </row>
-    <row r="120" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D120" s="19" t="s">
         <v>162</v>
       </c>
@@ -34070,7 +34070,7 @@
         <v>46.137865880580037</v>
       </c>
     </row>
-    <row r="121" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D121" s="19" t="s">
         <v>162</v>
       </c>
@@ -34081,7 +34081,7 @@
         <v>34.93812928869707</v>
       </c>
     </row>
-    <row r="122" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D122" s="19" t="s">
         <v>162</v>
       </c>
@@ -34092,7 +34092,7 @@
         <v>27.471638227441758</v>
       </c>
     </row>
-    <row r="123" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D123" s="19" t="s">
         <v>162</v>
       </c>
@@ -34103,7 +34103,7 @@
         <v>22.774089751023496</v>
       </c>
     </row>
-    <row r="124" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D124" s="19" t="s">
         <v>162</v>
       </c>
@@ -34114,7 +34114,7 @@
         <v>15.727767036396102</v>
       </c>
     </row>
-    <row r="125" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D125" s="19" t="s">
         <v>162</v>
       </c>
@@ -34125,7 +34125,7 @@
         <v>9.6596165622714754</v>
       </c>
     </row>
-    <row r="126" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D126" s="19" t="s">
         <v>162</v>
       </c>
@@ -34136,7 +34136,7 @@
         <v>8.2794492877500225</v>
       </c>
     </row>
-    <row r="127" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D127" s="19" t="s">
         <v>162</v>
       </c>
@@ -34147,7 +34147,7 @@
         <v>7.0735333286609636</v>
       </c>
     </row>
-    <row r="128" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D128" s="19" t="s">
         <v>162</v>
       </c>
@@ -34158,7 +34158,7 @@
         <v>5.2903275793547166</v>
       </c>
     </row>
-    <row r="129" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C129" s="19" t="str">
         <f>+D53</f>
         <v>MIN-P3-CAM6</v>
@@ -34177,7 +34177,7 @@
         <v>11.997774426540611</v>
       </c>
     </row>
-    <row r="130" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D130" s="19" t="s">
         <v>162</v>
       </c>
@@ -34188,7 +34188,7 @@
         <v>27.835107673690871</v>
       </c>
     </row>
-    <row r="131" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D131" s="19" t="s">
         <v>162</v>
       </c>
@@ -34199,7 +34199,7 @@
         <v>17.559909024325922</v>
       </c>
     </row>
-    <row r="132" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D132" s="19" t="s">
         <v>162</v>
       </c>
@@ -34210,7 +34210,7 @@
         <v>20.274712206938659</v>
       </c>
     </row>
-    <row r="133" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D133" s="19" t="s">
         <v>162</v>
       </c>
@@ -34221,7 +34221,7 @@
         <v>12.813096418110867</v>
       </c>
     </row>
-    <row r="134" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D134" s="19" t="s">
         <v>162</v>
       </c>
@@ -34232,7 +34232,7 @@
         <v>12.747595139993381</v>
       </c>
     </row>
-    <row r="135" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D135" s="19" t="s">
         <v>162</v>
       </c>
@@ -34243,7 +34243,7 @@
         <v>8.1699853499332526</v>
       </c>
     </row>
-    <row r="136" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D136" s="19" t="s">
         <v>162</v>
       </c>
@@ -34254,7 +34254,7 @@
         <v>8.8839477570677019</v>
       </c>
     </row>
-    <row r="137" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D137" s="19" t="s">
         <v>162</v>
       </c>
@@ -34265,7 +34265,7 @@
         <v>7.6545148810463139</v>
       </c>
     </row>
-    <row r="138" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D138" s="19" t="s">
         <v>162</v>
       </c>
@@ -34276,7 +34276,7 @@
         <v>5.5289075934361867</v>
       </c>
     </row>
-    <row r="139" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D139" s="19" t="s">
         <v>162</v>
       </c>
@@ -34287,7 +34287,7 @@
         <v>4.8075273037748882</v>
       </c>
     </row>
-    <row r="140" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D140" s="19" t="s">
         <v>162</v>
       </c>
@@ -34298,7 +34298,7 @@
         <v>4.3266071106673554</v>
       </c>
     </row>
-    <row r="141" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D141" s="19" t="s">
         <v>162</v>
       </c>
@@ -34309,7 +34309,7 @@
         <v>3.9981896052775268</v>
       </c>
     </row>
-    <row r="142" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D142" s="19" t="s">
         <v>162</v>
       </c>
@@ -34320,7 +34320,7 @@
         <v>3.5055633471927838</v>
       </c>
     </row>
-    <row r="143" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C143" s="19" t="str">
         <f>+D54</f>
         <v>MIN-P3-CAM7</v>
@@ -34339,7 +34339,7 @@
         <v>6.5119610393585514</v>
       </c>
     </row>
-    <row r="144" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D144" s="19" t="s">
         <v>162</v>
       </c>
@@ -34350,7 +34350,7 @@
         <v>13.481821376850158</v>
       </c>
     </row>
-    <row r="145" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D145" s="19" t="s">
         <v>162</v>
       </c>
@@ -34361,7 +34361,7 @@
         <v>13.508917511179082</v>
       </c>
     </row>
-    <row r="146" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D146" s="19" t="s">
         <v>162</v>
       </c>
@@ -34372,7 +34372,7 @@
         <v>11.452716398983046</v>
       </c>
     </row>
-    <row r="147" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D147" s="19" t="s">
         <v>162</v>
       </c>
@@ -34383,7 +34383,7 @@
         <v>9.7608949656530672</v>
       </c>
     </row>
-    <row r="148" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D148" s="19" t="s">
         <v>162</v>
       </c>
@@ -34394,7 +34394,7 @@
         <v>7.6571590031467025</v>
       </c>
     </row>
-    <row r="149" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D149" s="19" t="s">
         <v>162</v>
       </c>
@@ -34405,7 +34405,7 @@
         <v>6.1813413727745186</v>
       </c>
     </row>
-    <row r="150" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D150" s="19" t="s">
         <v>162</v>
       </c>
@@ -34416,7 +34416,7 @@
         <v>5.2908833074602128</v>
       </c>
     </row>
-    <row r="151" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D151" s="19" t="s">
         <v>162</v>
       </c>
@@ -34427,7 +34427,7 @@
         <v>4.5396783970548498</v>
       </c>
     </row>
-    <row r="152" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D152" s="19" t="s">
         <v>162</v>
       </c>
@@ -34438,7 +34438,7 @@
         <v>3.6489860397841127</v>
       </c>
     </row>
-    <row r="153" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D153" s="19" t="s">
         <v>162</v>
       </c>
@@ -34449,7 +34449,7 @@
         <v>0.66755939822291932</v>
       </c>
     </row>
-    <row r="154" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D154" s="19" t="s">
         <v>162</v>
       </c>
@@ -34460,7 +34460,7 @@
         <v>0.56675340398689622</v>
       </c>
     </row>
-    <row r="155" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D155" s="19" t="s">
         <v>162</v>
       </c>
@@ -34471,7 +34471,7 @@
         <v>0.48255766260835375</v>
       </c>
     </row>
-    <row r="156" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D156" s="19" t="s">
         <v>162</v>
       </c>

</xml_diff>